<commit_message>
filtrado por mes y punto
</commit_message>
<xml_diff>
--- a/servicios_adapta/tabla_mediciones.xlsx
+++ b/servicios_adapta/tabla_mediciones.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -491,21 +491,21 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>45022</v>
+        <v>45014</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>R1</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>16:09</t>
+          <t>14:35</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>16:24</t>
+          <t>14:50</t>
         </is>
       </c>
       <c r="E2" t="n">
@@ -515,15 +515,205 @@
         <v>1</v>
       </c>
       <c r="G2" t="n">
-        <v>68.59999999999999</v>
+        <v>64.7</v>
       </c>
       <c r="H2" t="n">
-        <v>71.90000000000001</v>
+        <v>65.59999999999999</v>
       </c>
       <c r="I2" t="n">
-        <v>59.3</v>
+        <v>63.1</v>
       </c>
       <c r="J2" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="n">
+        <v>45012</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>R3</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>20:17</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>20:32</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>15</v>
+      </c>
+      <c r="F3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" t="n">
+        <v>66.59999999999999</v>
+      </c>
+      <c r="H3" t="n">
+        <v>69.5</v>
+      </c>
+      <c r="I3" t="n">
+        <v>62.8</v>
+      </c>
+      <c r="J3" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="n">
+        <v>45007</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>R3</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>12:58</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>13:13</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>15</v>
+      </c>
+      <c r="F4" t="n">
+        <v>2</v>
+      </c>
+      <c r="G4" t="n">
+        <v>63.6</v>
+      </c>
+      <c r="H4" t="n">
+        <v>64.7</v>
+      </c>
+      <c r="I4" t="n">
+        <v>61.7</v>
+      </c>
+      <c r="J4" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="n">
+        <v>45006</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>R3</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>19:47</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>20:02</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>15</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" t="n">
+        <v>65.09999999999999</v>
+      </c>
+      <c r="H5" t="n">
+        <v>66.09999999999999</v>
+      </c>
+      <c r="I5" t="n">
+        <v>63.2</v>
+      </c>
+      <c r="J5" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="n">
+        <v>45002</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>R3</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>08:12</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>08:27</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>15</v>
+      </c>
+      <c r="F6" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" t="n">
+        <v>67.2</v>
+      </c>
+      <c r="H6" t="n">
+        <v>68.8</v>
+      </c>
+      <c r="I6" t="n">
+        <v>65.3</v>
+      </c>
+      <c r="J6" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="n">
+        <v>45001</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>R3</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>11:22</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>11:37</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>15</v>
+      </c>
+      <c r="F7" t="n">
+        <v>2</v>
+      </c>
+      <c r="G7" t="n">
+        <v>69.7</v>
+      </c>
+      <c r="H7" t="n">
+        <v>71.7</v>
+      </c>
+      <c r="I7" t="n">
+        <v>66.8</v>
+      </c>
+      <c r="J7" t="n">
         <v>75</v>
       </c>
     </row>

</xml_diff>

<commit_message>
solucion error por fracciones en tiempo
</commit_message>
<xml_diff>
--- a/servicios_adapta/tabla_mediciones.xlsx
+++ b/servicios_adapta/tabla_mediciones.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabla de Mediciones" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Tabla de Mediciones" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>